<commit_message>
AIP-494 AIP-790 Updated Test Data File
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_731.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_731.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C716A756-593D-41E6-BC7E-CB9067E4177A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF3546B-9542-4E52-BC03-8CA4AD3F9B22}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>DeviceName</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>700</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +554,106 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>